<commit_message>
remove bugs and update code with special character and 30 character lenght
</commit_message>
<xml_diff>
--- a/processed/SCHCT_31.03.2025_vendor_list_SBI_Gorhe.xlsx
+++ b/processed/SCHCT_31.03.2025_vendor_list_SBI_Gorhe.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1522,318 +1522,24 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>404985</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>O|A|nan|nan||nan|nan|nan|India</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr"/>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>O|A|nan|nan||nan|nan|nan|India</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="inlineStr"/>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>O|A|nan|nan||nan|nan|nan|India</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr"/>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>O|A|nan|nan||nan|nan|nan|India</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr"/>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="inlineStr"/>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>O|A|nan|nan||nan|nan|nan|India</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr"/>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>O|A|nan|nan||nan|nan|nan|India</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>  </t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="inlineStr"/>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>India</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>O|A|nan|  ||nan|nan|nan|India</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>404985</v>
-      </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="inlineStr"/>
-      <c r="K28" t="inlineStr"/>
-      <c r="L28" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>